<commit_message>
UC03, UC04, UC05 documentation
</commit_message>
<xml_diff>
--- a/UseCasesDescriptions/UseCasesDescription.xlsx
+++ b/UseCasesDescriptions/UseCasesDescription.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation\TeamPRO\UseCasesDescriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6AAA63-24D2-4E04-B44E-1B5AD9D20F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3FF828-061D-460A-866A-D05D895E9E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8EA4B9D8-8AA4-46FC-8FF3-1CA2ECB712B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8EA4B9D8-8AA4-46FC-8FF3-1CA2ECB712B4}"/>
   </bookViews>
   <sheets>
     <sheet name="UC01 - Login" sheetId="1" r:id="rId1"/>
     <sheet name="UC02 - Create a team" sheetId="2" r:id="rId2"/>
+    <sheet name="UC03 - Join a team" sheetId="3" r:id="rId3"/>
+    <sheet name="UC04 - Resign from a team" sheetId="4" r:id="rId4"/>
+    <sheet name="UC05 - See all active membersh" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t xml:space="preserve">Use-Case name </t>
   </si>
@@ -115,6 +118,63 @@
   </si>
   <si>
     <t>This use-case describes how to create a new team</t>
+  </si>
+  <si>
+    <t>This use-case describes how to join a team</t>
+  </si>
+  <si>
+    <t>UC03 - Join a team</t>
+  </si>
+  <si>
+    <t>2. Select one of the teams available</t>
+  </si>
+  <si>
+    <t>5. Confirm the operation</t>
+  </si>
+  <si>
+    <t>7. Show team page updated with the new membership</t>
+  </si>
+  <si>
+    <t>3. Redirect to the selected team page</t>
+  </si>
+  <si>
+    <t>UC04 - Resign from a team</t>
+  </si>
+  <si>
+    <t>This use-case describes how to resign from a team</t>
+  </si>
+  <si>
+    <t>2. Click on the team they want to resign from</t>
+  </si>
+  <si>
+    <t>4. Click the "Leave team" option</t>
+  </si>
+  <si>
+    <t>4. Click on an open position</t>
+  </si>
+  <si>
+    <t>UC05 - See all active memberships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athlete </t>
+  </si>
+  <si>
+    <t>The athlete must have an account</t>
+  </si>
+  <si>
+    <t>Athlete must have previously joined the team</t>
+  </si>
+  <si>
+    <t>6. Unbind the athlete from the team</t>
+  </si>
+  <si>
+    <t>7. Redirects athlete to their home page</t>
+  </si>
+  <si>
+    <t>2. Show all teams the athlete belongs to</t>
+  </si>
+  <si>
+    <t>6. Bind the athlete to the team</t>
   </si>
 </sst>
 </file>
@@ -627,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18B358E-5483-44BF-8E19-4B6AF75E9EAD}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,4 +800,337 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC2861A2-C9D1-4BF5-93AF-347C72BDDCDB}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FADC539-654C-450F-B115-45B381986D61}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87534CEC-6720-4079-A05B-CFB88F1C951B}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>